<commit_message>
Practical Record for unit 1
</commit_message>
<xml_diff>
--- a/php program List.xlsx
+++ b/php program List.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$38</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="38">
   <si>
     <t>S.No</t>
   </si>
@@ -47,9 +50,6 @@
     <t>Arm Strong or not</t>
   </si>
   <si>
-    <t>Generation of ArmStrong Numbers ]</t>
-  </si>
-  <si>
     <t xml:space="preserve">Product of Prime </t>
   </si>
   <si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>Generation of ArmStrong Numbers</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -166,7 +172,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -189,11 +195,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -212,6 +227,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -493,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,226 +525,238 @@
     <col min="4" max="4" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="8"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -733,10 +764,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" s="5"/>
     </row>
@@ -745,10 +776,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" s="5"/>
     </row>
@@ -757,13 +788,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -771,13 +802,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -785,10 +816,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D21" s="5"/>
     </row>
@@ -797,10 +828,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D22" s="5"/>
     </row>
@@ -809,13 +840,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -823,13 +854,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -837,13 +868,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -851,13 +882,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -865,13 +896,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -879,13 +910,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -893,10 +924,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D29" s="5"/>
     </row>

</xml_diff>